<commit_message>
Finally the project started running
</commit_message>
<xml_diff>
--- a/IdentifyCourses.Coursera.org/target/test-classes/Count_Of_Languages.xlsx
+++ b/IdentifyCourses.Coursera.org/target/test-classes/Count_Of_Languages.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408293\git\Team_ChatureBhature_IdentifyCourses\IdentifyCourses.Coursera.org\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408354\git\Team_ChatureBhature_IdentifyCourses\IdentifyCourses.Coursera.org\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58266DE1-1AE8-4D2C-8893-10A6DB8C4771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB538D4E-83FF-4911-8047-7A87E6268A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E2ACAEC7-E164-4C10-81D1-F69421976CEC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="32">
   <si>
     <t>Languages And Count</t>
   </si>
@@ -504,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5447F97-9D47-40AC-AE8E-7981387DE99A}">
-  <dimension ref="A1:A63"/>
+  <dimension ref="A1:A404"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="A1:XFD1048576"/>
@@ -827,6 +827,1711 @@
         <v>31</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Deleted duplicated xlsx file
</commit_message>
<xml_diff>
--- a/IdentifyCourses.Coursera.org/target/test-classes/Count_Of_Languages.xlsx
+++ b/IdentifyCourses.Coursera.org/target/test-classes/Count_Of_Languages.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408293\git\Team_ChatureBhature_IdentifyCourses\IdentifyCourses.Coursera.org\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673434F0-4B09-429F-9663-1B101B55BDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBB2974-7958-49E2-810D-710CBDA6255D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E2ACAEC7-E164-4C10-81D1-F69421976CEC}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -138,7 +138,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -512,163 +511,163 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s" s="0">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s" s="0">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s" s="0">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s" s="0">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s" s="0">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s" s="0">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s" s="0">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="s" s="0">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="s" s="0">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="s" s="0">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="s" s="0">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="s" s="0">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="s" s="0">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="s" s="0">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>